<commit_message>
added 3yr baseline data
</commit_message>
<xml_diff>
--- a/code/Jichong/moduel_dictionary_models.xlsx
+++ b/code/Jichong/moduel_dictionary_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb576802\Documents\non-work\GWU\Capstone\Github folders\Capstone\code\Jichong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C6A9C-C126-4199-A2AE-3C4F1C209EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A476730-3163-40D9-BE0F-E6784E267106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2F449D38-8939-4DD5-8418-8E65FDF5F64A}"/>
+    <workbookView xWindow="57480" yWindow="-2835" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2F449D38-8939-4DD5-8418-8E65FDF5F64A}"/>
   </bookViews>
   <sheets>
     <sheet name="Option3" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="106">
   <si>
     <t>Class</t>
   </si>
@@ -327,10 +327,58 @@
     <t>featuretools</t>
   </si>
   <si>
-    <t>Class - feature engineering</t>
-  </si>
-  <si>
     <t>PCA</t>
+  </si>
+  <si>
+    <t>class - data pre-processing</t>
+  </si>
+  <si>
+    <t>class - baseline models</t>
+  </si>
+  <si>
+    <t>class - feature selection</t>
+  </si>
+  <si>
+    <t>class - feature engineering</t>
+  </si>
+  <si>
+    <t>utility</t>
+  </si>
+  <si>
+    <t>file_compare()</t>
+  </si>
+  <si>
+    <t>glossary()</t>
+  </si>
+  <si>
+    <t>datasci</t>
+  </si>
+  <si>
+    <t>.size()</t>
+  </si>
+  <si>
+    <t>.recode()</t>
+  </si>
+  <si>
+    <t>.missingReport()</t>
+  </si>
+  <si>
+    <t>.remove_all_nan_columns()</t>
+  </si>
+  <si>
+    <t>.impute_all()</t>
+  </si>
+  <si>
+    <t>.imputation()</t>
+  </si>
+  <si>
+    <t>.standardize()</t>
+  </si>
+  <si>
+    <t>.eda()</t>
+  </si>
+  <si>
+    <t>.featureSelection()</t>
   </si>
 </sst>
 </file>
@@ -412,7 +460,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +521,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -495,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -604,7 +676,19 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -622,19 +706,22 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -956,37 +1043,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="2" customFormat="1" ht="15.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52" t="s">
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="49" t="s">
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="53" t="s">
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" ht="15.5">
       <c r="A2" s="20" t="s">
@@ -2976,16 +3063,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="15.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="49" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="15.5">
       <c r="A2" s="4" t="s">
@@ -3783,15 +3870,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="15.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="49" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="49"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="15.5">
       <c r="A2" s="4" t="s">
@@ -4593,817 +4680,872 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="32.08203125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="26.75" style="38" customWidth="1"/>
-    <col min="5" max="5" width="39.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="31"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.9140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="32.08203125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="26.75" style="38" customWidth="1"/>
+    <col min="7" max="7" width="39.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.5">
-      <c r="A1" s="46"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="57"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.5">
-      <c r="A2" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="47" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15.5">
+      <c r="A1" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="58"/>
+      <c r="F1" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15.5">
+      <c r="A2" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="51"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="14">
+      <c r="A3" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="57"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="15.5">
-      <c r="A3" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="28" t="s">
+      <c r="E3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="57"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="28" t="s">
+      <c r="G3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="51"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="52"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="28" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F5" s="28"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="28"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="28" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28" t="s">
-        <v>47</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="28" t="s">
+      <c r="H8" s="52"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="35"/>
+      <c r="G9" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="28" t="s">
+      <c r="H9" s="52"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="28" t="s">
+      <c r="H10" s="28"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="28" t="s">
+      <c r="H11" s="52"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="28" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="28" t="s">
+      <c r="H13" s="52"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="28" t="s">
+      <c r="H14" s="52"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="28" t="s">
+      <c r="H15" s="52"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="28" t="s">
+      <c r="H16" s="52"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="3:11">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="28" t="s">
+      <c r="H17" s="52"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="3:11">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="58"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="28" t="s">
+      <c r="H18" s="52"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="3:11">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="58"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="28" t="s">
+      <c r="H19" s="52"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="3:11">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="58"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="28" t="s">
+      <c r="H20" s="52"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="3:11">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="58"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="52"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="54"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="3:11">
+      <c r="C22" s="18"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="52"/>
       <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="54"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="3:11">
+      <c r="C23" s="18"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="52"/>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="54"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="3:11">
+      <c r="C24" s="18"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="52"/>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="54"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="3:11">
+      <c r="C25" s="18"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="52"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="54"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="3:11">
+      <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="52"/>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="54"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="3:11">
+      <c r="C27" s="18"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="52"/>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="54"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="3:11">
+      <c r="C28" s="18"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="52"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="54"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="3:11">
+      <c r="C29" s="18"/>
       <c r="D29" s="18"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="52"/>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="54"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="3:11">
+      <c r="C30" s="18"/>
       <c r="D30" s="18"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="52"/>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="54"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="3:11">
+      <c r="C31" s="18"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="52"/>
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="54"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="3:11">
+      <c r="C32" s="18"/>
       <c r="D32" s="18"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="52"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="54"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="3:11">
+      <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="52"/>
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="54"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="3:11">
+      <c r="C34" s="18"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="52"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="54"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="3:11">
+      <c r="C35" s="18"/>
       <c r="D35" s="18"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="52"/>
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="54"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="3:11">
+      <c r="C36" s="18"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="52"/>
       <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="54"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="3:11">
+      <c r="C37" s="18"/>
       <c r="D37" s="18"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="52"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="54"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="3:11">
+      <c r="C38" s="18"/>
       <c r="D38" s="18"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="52"/>
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="54"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="3:11">
+      <c r="C39" s="18"/>
       <c r="D39" s="18"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="52"/>
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="54"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="3:11">
+      <c r="C40" s="18"/>
       <c r="D40" s="18"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="52"/>
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="54"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="3:11">
+      <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="52"/>
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="54"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="3:11">
+      <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="52"/>
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="54"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="3:11">
+      <c r="C43" s="18"/>
       <c r="D43" s="18"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="52"/>
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="54"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="3:11">
+      <c r="C44" s="18"/>
       <c r="D44" s="18"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="52"/>
       <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="3:11">
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="52"/>
       <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="3:11">
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="52"/>
       <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="3:11">
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="52"/>
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="3:11">
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="52"/>
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="3:11">
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="52"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="3:11">
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="52"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="3:11">
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="52"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="22">
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="3:11">
+      <c r="C52" s="22">
         <v>6</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="52"/>
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="3:11">
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="52"/>
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="3:11">
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="52"/>
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="3:11">
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="52"/>
       <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="3:11">
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="52"/>
       <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="3:11">
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="52"/>
       <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="3:11">
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="52"/>
       <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="3:11">
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="52"/>
       <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="56"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="3:11">
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="52"/>
       <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="21">
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="3:11">
+      <c r="C61" s="21">
         <v>7</v>
       </c>
-      <c r="D61" s="37"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
       <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="D62" s="37"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="58"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="3:11">
+      <c r="F62" s="37"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
       <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="D63" s="37"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="3:11">
+      <c r="F63" s="37"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
       <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="D64" s="37"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="58"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="3:11">
+      <c r="F64" s="37"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="52"/>
       <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="4:9">
-      <c r="D65" s="37"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="6:11">
+      <c r="F65" s="37"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
       <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="4:9">
-      <c r="D66" s="37"/>
-    </row>
-    <row r="67" spans="4:9">
-      <c r="D67" s="37"/>
-    </row>
-    <row r="68" spans="4:9">
-      <c r="D68" s="37"/>
-    </row>
-    <row r="69" spans="4:9">
-      <c r="D69" s="37"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+    </row>
+    <row r="66" spans="6:11">
+      <c r="F66" s="37"/>
+    </row>
+    <row r="67" spans="6:11">
+      <c r="F67" s="37"/>
+    </row>
+    <row r="68" spans="6:11">
+      <c r="F68" s="37"/>
+    </row>
+    <row r="69" spans="6:11">
+      <c r="F69" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>